<commit_message>
Added option to write binary rrgraph
</commit_message>
<xml_diff>
--- a/examples/OpenFPGA_basic/baseline_l4/switchbox_left.xlsx
+++ b/examples/OpenFPGA_basic/baseline_l4/switchbox_left.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Right</t>
   </si>
@@ -85,7 +85,7 @@
     <t>io_left[19].f2a_i[0]</t>
   </si>
   <si>
-    <t/>
+    <t>X</t>
   </si>
   <si>
     <t>OPIN</t>
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -258,9 +258,6 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -584,46 +581,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="13" width="5.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="13" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="14" width="3.7192857142857143" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="28" max="28" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="35" max="35" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="36" max="36" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="37" max="37" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="38" max="38" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="39" max="39" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="40" max="40" style="14" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="10" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="11" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="5.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="12" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="13" width="3.7192857142857143" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="13" width="8.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -1071,7 +1068,7 @@
       <c r="D6" s="4">
         <v>1</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="F6" s="5"/>
@@ -1085,9 +1082,7 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -1125,21 +1120,15 @@
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
-      <c r="G7" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="K7" s="5"/>
       <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
-      <c r="O7" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="O7" s="5"/>
       <c r="P7" s="5"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="5"/>
@@ -1237,9 +1226,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
@@ -1809,9 +1796,7 @@
       <c r="D21" s="4">
         <v>4</v>
       </c>
-      <c r="E21" s="10" t="s">
-        <v>23</v>
-      </c>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>

</xml_diff>